<commit_message>
Atualização automática de SANTO_CRISTO.xlsx
</commit_message>
<xml_diff>
--- a/SANTO_CRISTO.xlsx
+++ b/SANTO_CRISTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C94A7E58-00E2-4224-9809-6490D1A51876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E221F6-4A62-4D02-9A20-4635EF3003EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,7 +1288,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{4B2F9921-FD58-4EF0-B962-4479D4640556}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{CC302D06-1B41-4C1A-B31E-C7DCDF43D494}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1318,10 +1318,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B2985B-D63B-4A43-80B0-62C9FBCEE2A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EBAB18F-35DF-416C-87B8-F1C7DA14ECC9}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D56186-0734-43CF-A029-E28FF1AF0A3D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C61FB09A-6ECE-45A8-8DDE-DF563DBF90B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3E6EEA9-8D16-4BED-B3DA-97EF002D4B0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D033C3E-7C08-43DE-B71D-493BE706ED63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1441,7 +1441,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B529E8F-9828-E9B9-EB3B-A145CCFB419C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2D22AB6-0EF5-54A0-0FDD-A496B2735644}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A251B43F-57F8-7AB0-BF83-ED9A377CFFA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD8D6AF-5EB3-FD01-9FE9-0F0E887AC198}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1509,7 +1509,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020939CC-AF0D-D1B9-98A6-8EF99CD95BE3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AABE7B8A-7514-5027-B4D8-322CC0C15556}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1540,7 +1540,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C35B8383-3CFE-24F4-F82F-D151309DB676}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{185609C3-BCA0-3021-2609-D4C89A4CFBD1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1571,7 +1571,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D90182A-69E5-EC40-2A52-B9DB2741CB0D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1D8AD5D-BCA7-1247-7841-35F423886DF7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1614,7 +1614,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F780E69-D46B-421E-B194-8FBE31FB50F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A50B45-9998-44EC-B7B0-376B033FA30A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1652,7 +1652,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC4001B-A966-430B-9FED-DCAA93DC3364}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED97331-2517-4C76-A2A2-93553FAA6F1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,7 +1695,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CBB5773-78D2-47FC-BF67-F6E36828CA22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5775D9A-FD11-4CAA-8F50-A5E88B9432D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,7 +2008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F190C0-F375-4ACE-8950-2AE95A0690B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83136FA7-DEAE-459F-A12C-EA9764C1F81C}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>